<commit_message>
add new vars & new v2 file
</commit_message>
<xml_diff>
--- a/data/11/aud_use_week.xlsx
+++ b/data/11/aud_use_week.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seungmi/workspace/studying/bigcon_mmmz/master/data/11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADCA510-69CD-F445-A9C4-836D2F8E57D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26E93B9-21AD-1947-B2F1-9E3107DFA125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="0" windowWidth="27980" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="0" windowWidth="27920" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="329">
   <si>
     <t>6:00</t>
   </si>
@@ -280,9 +280,6 @@
     <t>4.7</t>
   </si>
   <si>
-    <t>이상</t>
-  </si>
-  <si>
     <t>3.4</t>
   </si>
   <si>
@@ -469,9 +466,6 @@
     <t>21.3</t>
   </si>
   <si>
-    <t>33.1</t>
-  </si>
-  <si>
     <t>12.8</t>
   </si>
   <si>
@@ -490,9 +484,6 @@
     <t>19.2</t>
   </si>
   <si>
-    <t>32.1 30.9</t>
-  </si>
-  <si>
     <t>10.3</t>
   </si>
   <si>
@@ -607,9 +598,6 @@
     <t>10.4</t>
   </si>
   <si>
-    <t>10.3 9.5</t>
-  </si>
-  <si>
     <t>7.7</t>
   </si>
   <si>
@@ -679,9 +667,6 @@
     <t>16.6</t>
   </si>
   <si>
-    <t>17.1 16.6</t>
-  </si>
-  <si>
     <t>9.4</t>
   </si>
   <si>
@@ -883,9 +868,6 @@
     <t>61.9</t>
   </si>
   <si>
-    <t>62.0 58.7</t>
-  </si>
-  <si>
     <t>43.9</t>
   </si>
   <si>
@@ -1018,9 +1000,6 @@
     <t>1.7</t>
   </si>
   <si>
-    <t>1.2 1.2</t>
-  </si>
-  <si>
     <t>0.2</t>
   </si>
   <si>
@@ -1028,9 +1007,6 @@
   </si>
   <si>
     <t>0.4</t>
-  </si>
-  <si>
-    <t>0.5 0.5</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1042,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1385,7 +1363,7 @@
   <dimension ref="A1:BU9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1616,217 +1594,217 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="N2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="P2" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q2" t="s">
         <v>167</v>
       </c>
-      <c r="Q2" t="s">
-        <v>170</v>
-      </c>
       <c r="R2" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" t="s">
+        <v>176</v>
+      </c>
+      <c r="T2" t="s">
+        <v>173</v>
+      </c>
+      <c r="U2" t="s">
+        <v>167</v>
+      </c>
+      <c r="V2" t="s">
+        <v>184</v>
+      </c>
+      <c r="W2" t="s">
         <v>174</v>
       </c>
-      <c r="S2" t="s">
-        <v>179</v>
-      </c>
-      <c r="T2" t="s">
-        <v>176</v>
-      </c>
-      <c r="U2" t="s">
-        <v>170</v>
-      </c>
-      <c r="V2" t="s">
-        <v>187</v>
-      </c>
-      <c r="W2" t="s">
-        <v>177</v>
-      </c>
       <c r="X2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Y2" t="s">
         <v>85</v>
       </c>
       <c r="Z2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AA2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AB2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="AC2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AD2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="AE2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="AF2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AG2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>181</v>
+      </c>
+      <c r="AL2" t="s">
         <v>159</v>
       </c>
-      <c r="AH2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>162</v>
-      </c>
       <c r="AM2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="AN2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="AO2" t="s">
+        <v>223</v>
+      </c>
+      <c r="AP2" t="s">
         <v>228</v>
       </c>
-      <c r="AP2" t="s">
-        <v>233</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="AR2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="AS2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="AT2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="AU2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="AV2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="AW2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="AX2" t="s">
+        <v>282</v>
+      </c>
+      <c r="AY2" t="s">
         <v>288</v>
       </c>
-      <c r="AY2" t="s">
-        <v>294</v>
-      </c>
       <c r="AZ2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="BA2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="BB2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="BC2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="BD2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="BE2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="BF2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="BG2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="BH2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="BI2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="BJ2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BK2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BL2" t="s">
         <v>82</v>
       </c>
       <c r="BM2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BN2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BO2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BP2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BQ2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BR2" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BS2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BT2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BU2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.2">
@@ -1843,184 +1821,184 @@
         <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J3" t="s">
         <v>83</v>
       </c>
       <c r="K3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="O3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P3" t="s">
         <v>85</v>
       </c>
       <c r="Q3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="R3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="S3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="T3" t="s">
         <v>85</v>
       </c>
       <c r="U3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="W3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="X3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Y3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Z3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AA3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AB3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AC3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AD3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AE3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AF3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH3" t="s">
         <v>208</v>
       </c>
-      <c r="AG3" t="s">
-        <v>208</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>212</v>
-      </c>
       <c r="AI3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AL3" t="s">
         <v>202</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>202</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>202</v>
-      </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>152</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>229</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>236</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>242</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>238</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>249</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>270</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>277</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>283</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>232</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>296</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>124</v>
+      </c>
+      <c r="BC3" t="s">
         <v>206</v>
       </c>
-      <c r="AM3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>225</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>234</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>241</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>247</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>125</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>243</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>254</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>275</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>282</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>289</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>237</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>302</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>125</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>125</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>210</v>
-      </c>
       <c r="BD3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="BE3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BF3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="BG3" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="BH3" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BI3" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BJ3" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BK3" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BL3" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BM3" t="s">
         <v>81</v>
@@ -2041,13 +2019,13 @@
         <v>81</v>
       </c>
       <c r="BS3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BT3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BU3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.2">
@@ -2058,190 +2036,190 @@
         <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N4" t="s">
+        <v>156</v>
+      </c>
+      <c r="O4" t="s">
+        <v>114</v>
+      </c>
+      <c r="P4" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>134</v>
+      </c>
+      <c r="R4" t="s">
+        <v>173</v>
+      </c>
+      <c r="S4" t="s">
+        <v>173</v>
+      </c>
+      <c r="T4" t="s">
+        <v>114</v>
+      </c>
+      <c r="U4" t="s">
+        <v>181</v>
+      </c>
+      <c r="V4" t="s">
+        <v>185</v>
+      </c>
+      <c r="W4" t="s">
+        <v>189</v>
+      </c>
+      <c r="X4" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Z4" t="s">
         <v>94</v>
       </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G4" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" t="s">
-        <v>146</v>
-      </c>
-      <c r="M4" t="s">
-        <v>152</v>
-      </c>
-      <c r="N4" t="s">
-        <v>159</v>
-      </c>
-      <c r="O4" t="s">
-        <v>115</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="AA4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB4" t="s">
         <v>168</v>
       </c>
-      <c r="Q4" t="s">
-        <v>135</v>
-      </c>
-      <c r="R4" t="s">
-        <v>176</v>
-      </c>
-      <c r="S4" t="s">
-        <v>176</v>
-      </c>
-      <c r="T4" t="s">
-        <v>115</v>
-      </c>
-      <c r="U4" t="s">
-        <v>184</v>
-      </c>
-      <c r="V4" t="s">
-        <v>188</v>
-      </c>
-      <c r="W4" t="s">
-        <v>192</v>
-      </c>
-      <c r="X4" t="s">
-        <v>192</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>188</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>171</v>
-      </c>
       <c r="AC4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE4" t="s">
         <v>201</v>
       </c>
-      <c r="AD4" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>205</v>
-      </c>
       <c r="AF4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="AG4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AH4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="AI4" t="s">
         <v>85</v>
       </c>
       <c r="AJ4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AK4" t="s">
         <v>85</v>
       </c>
       <c r="AL4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AM4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AN4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AO4" t="s">
+        <v>200</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>237</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>249</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>256</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>241</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>278</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>284</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>289</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>297</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>302</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>308</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>312</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>225</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>207</v>
+      </c>
+      <c r="BH4" t="s">
         <v>204</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>218</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>242</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>138</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>261</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>268</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>246</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>283</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>290</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>295</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>303</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>308</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>314</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>318</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>230</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>224</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>211</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>208</v>
       </c>
       <c r="BI4" t="s">
         <v>84</v>
       </c>
       <c r="BJ4" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="BK4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BL4" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="BM4" t="s">
         <v>82</v>
@@ -2285,61 +2263,61 @@
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="R5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="S5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="T5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="U5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="V5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="W5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X5" t="s">
         <v>83</v>
@@ -2348,112 +2326,112 @@
         <v>80</v>
       </c>
       <c r="Z5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AA5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AB5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="AD5" t="s">
         <v>85</v>
       </c>
       <c r="AE5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="AF5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="AH5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AI5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AJ5" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="AK5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AL5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AM5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AO5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="AP5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="AQ5" t="s">
+        <v>238</v>
+      </c>
+      <c r="AR5" t="s">
         <v>243</v>
       </c>
-      <c r="AR5" t="s">
-        <v>248</v>
-      </c>
       <c r="AS5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="AT5" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="AU5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="AV5" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="AW5" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="AX5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="AY5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="AZ5" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="BA5" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="BB5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="BC5" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="BD5" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="BE5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BF5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="BG5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="BH5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="BI5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BJ5" t="s">
         <v>82</v>
@@ -2465,13 +2443,13 @@
         <v>82</v>
       </c>
       <c r="BM5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BN5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BO5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BP5" t="s">
         <v>81</v>
@@ -2483,10 +2461,10 @@
         <v>81</v>
       </c>
       <c r="BS5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BT5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BU5" t="s">
         <v>82</v>
@@ -2500,67 +2478,67 @@
         <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" t="s">
+        <v>141</v>
+      </c>
+      <c r="L6" t="s">
+        <v>102</v>
+      </c>
+      <c r="M6" t="s">
+        <v>152</v>
+      </c>
+      <c r="N6" t="s">
+        <v>157</v>
+      </c>
+      <c r="O6" t="s">
+        <v>161</v>
+      </c>
+      <c r="P6" t="s">
         <v>95</v>
       </c>
-      <c r="E6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H6" t="s">
-        <v>124</v>
-      </c>
-      <c r="I6" t="s">
-        <v>130</v>
-      </c>
-      <c r="J6" t="s">
-        <v>136</v>
-      </c>
-      <c r="K6" t="s">
-        <v>142</v>
-      </c>
-      <c r="L6" t="s">
-        <v>103</v>
-      </c>
-      <c r="M6" t="s">
-        <v>154</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="Q6" t="s">
+        <v>156</v>
+      </c>
+      <c r="R6" t="s">
+        <v>114</v>
+      </c>
+      <c r="S6" t="s">
+        <v>134</v>
+      </c>
+      <c r="T6" t="s">
+        <v>174</v>
+      </c>
+      <c r="U6" t="s">
+        <v>182</v>
+      </c>
+      <c r="V6" t="s">
         <v>160</v>
       </c>
-      <c r="O6" t="s">
-        <v>164</v>
-      </c>
-      <c r="P6" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>159</v>
-      </c>
-      <c r="R6" t="s">
-        <v>115</v>
-      </c>
-      <c r="S6" t="s">
-        <v>135</v>
-      </c>
-      <c r="T6" t="s">
-        <v>177</v>
-      </c>
-      <c r="U6" t="s">
-        <v>185</v>
-      </c>
-      <c r="V6" t="s">
-        <v>163</v>
-      </c>
       <c r="W6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X6" t="s">
         <v>83</v>
@@ -2569,130 +2547,130 @@
         <v>84</v>
       </c>
       <c r="Z6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AA6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AB6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AC6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AD6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AE6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AF6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="AG6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AH6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AI6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AJ6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="AK6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AL6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="AM6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AN6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AO6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="AP6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AQ6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="AR6" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="AS6" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="AT6" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="AU6" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="AV6" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="AW6" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="AX6" t="s">
+        <v>285</v>
+      </c>
+      <c r="AY6" t="s">
         <v>291</v>
       </c>
-      <c r="AY6" t="s">
-        <v>297</v>
-      </c>
       <c r="AZ6" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="BA6" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="BB6" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="BC6" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="BD6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="BE6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="BF6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG6" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="BH6" t="s">
         <v>84</v>
       </c>
       <c r="BI6" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="BJ6" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="BK6" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="BL6" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="BM6" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BN6" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BO6" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BP6" t="s">
         <v>81</v>
@@ -2721,208 +2699,208 @@
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" t="s">
+        <v>136</v>
+      </c>
+      <c r="K7" s="1">
+        <v>13.7</v>
+      </c>
+      <c r="L7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M7" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" t="s">
+        <v>158</v>
+      </c>
+      <c r="O7" t="s">
+        <v>162</v>
+      </c>
+      <c r="P7" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>122</v>
+      </c>
+      <c r="R7" t="s">
+        <v>175</v>
+      </c>
+      <c r="S7" t="s">
         <v>95</v>
       </c>
-      <c r="E7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I7" t="s">
-        <v>131</v>
-      </c>
-      <c r="J7" t="s">
-        <v>137</v>
-      </c>
-      <c r="K7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L7" t="s">
-        <v>147</v>
-      </c>
-      <c r="M7" t="s">
-        <v>106</v>
-      </c>
-      <c r="N7" t="s">
-        <v>161</v>
-      </c>
-      <c r="O7" t="s">
-        <v>165</v>
-      </c>
-      <c r="P7" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>123</v>
-      </c>
-      <c r="R7" t="s">
-        <v>178</v>
-      </c>
-      <c r="S7" t="s">
-        <v>96</v>
-      </c>
       <c r="T7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="U7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V7" t="s">
+        <v>186</v>
+      </c>
+      <c r="W7" t="s">
+        <v>190</v>
+      </c>
+      <c r="X7" t="s">
         <v>189</v>
       </c>
-      <c r="W7" t="s">
-        <v>193</v>
-      </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z7" t="s">
         <v>192</v>
       </c>
-      <c r="Y7" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>196</v>
-      </c>
       <c r="AA7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AB7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>192</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>134</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>215</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>191</v>
+      </c>
+      <c r="AN7" t="s">
         <v>152</v>
       </c>
-      <c r="AC7" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>178</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>196</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>96</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>174</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>115</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>135</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>198</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>220</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>194</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>154</v>
-      </c>
       <c r="AO7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AP7" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="AQ7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="AR7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="AS7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="AT7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="AU7" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="AV7" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="AW7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="AX7" t="s">
+        <v>286</v>
+      </c>
+      <c r="AY7" t="s">
         <v>292</v>
       </c>
-      <c r="AY7" t="s">
-        <v>298</v>
-      </c>
       <c r="AZ7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="BA7" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="BB7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="BC7" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="BD7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="BE7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="BF7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="BG7" t="s">
+        <v>320</v>
+      </c>
+      <c r="BH7" t="s">
+        <v>320</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>87</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL7" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM7" t="s">
         <v>326</v>
       </c>
-      <c r="BH7" t="s">
+      <c r="BN7" t="s">
         <v>326</v>
       </c>
-      <c r="BI7" t="s">
-        <v>94</v>
-      </c>
-      <c r="BJ7" t="s">
-        <v>88</v>
-      </c>
-      <c r="BK7" t="s">
-        <v>88</v>
-      </c>
-      <c r="BL7" t="s">
-        <v>88</v>
-      </c>
-      <c r="BM7" t="s">
-        <v>333</v>
-      </c>
-      <c r="BN7" t="s">
-        <v>333</v>
-      </c>
       <c r="BO7" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="BP7" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BQ7" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BR7" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BS7" t="s">
         <v>81</v>
@@ -2938,220 +2916,220 @@
       <c r="A8" t="s">
         <v>78</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J8" s="1">
+        <v>24.7</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" t="s">
-        <v>119</v>
-      </c>
-      <c r="H8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I8" t="s">
-        <v>132</v>
-      </c>
-      <c r="J8" t="s">
-        <v>138</v>
-      </c>
-      <c r="K8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L8" t="s">
-        <v>148</v>
-      </c>
-      <c r="M8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N8" t="s">
-        <v>162</v>
-      </c>
-      <c r="O8" t="s">
-        <v>106</v>
-      </c>
-      <c r="P8" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>172</v>
-      </c>
-      <c r="R8" t="s">
-        <v>172</v>
-      </c>
-      <c r="S8" t="s">
-        <v>172</v>
-      </c>
-      <c r="T8" t="s">
-        <v>182</v>
-      </c>
-      <c r="U8" t="s">
-        <v>92</v>
-      </c>
-      <c r="V8" t="s">
-        <v>108</v>
-      </c>
-      <c r="W8" t="s">
-        <v>187</v>
-      </c>
-      <c r="X8" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>187</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF8" t="s">
+      <c r="V8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="AG8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>116</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>167</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>217</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>217</v>
-      </c>
-      <c r="AL8" t="s">
+      <c r="AE8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AK8" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AL8" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AN8" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="AM8" t="s">
-        <v>173</v>
-      </c>
-      <c r="AN8" t="s">
+      <c r="AO8" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AO8" t="s">
-        <v>231</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>238</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>244</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>251</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>258</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>265</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>272</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>279</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>286</v>
-      </c>
-      <c r="AX8" t="s">
+      <c r="AP8" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AQ8" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="AR8" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="AS8" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="AT8" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="AU8" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="AV8" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="AW8" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="AX8" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AY8" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="AY8" t="s">
-        <v>299</v>
-      </c>
-      <c r="AZ8" t="s">
-        <v>306</v>
-      </c>
-      <c r="BA8" t="s">
-        <v>166</v>
-      </c>
-      <c r="BB8" t="s">
+      <c r="AZ8" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="BA8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BB8" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="BC8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="BE8" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="BC8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BD8" t="s">
-        <v>188</v>
-      </c>
-      <c r="BE8" t="s">
+      <c r="BF8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BG8" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="BH8" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="BF8" t="s">
+      <c r="BI8" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="BJ8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="BG8" t="s">
-        <v>327</v>
-      </c>
-      <c r="BH8" t="s">
-        <v>329</v>
-      </c>
-      <c r="BI8" t="s">
-        <v>329</v>
-      </c>
-      <c r="BJ8" t="s">
-        <v>88</v>
-      </c>
-      <c r="BK8" t="s">
-        <v>88</v>
-      </c>
-      <c r="BL8" t="s">
-        <v>88</v>
-      </c>
-      <c r="BM8" t="s">
-        <v>333</v>
-      </c>
-      <c r="BN8" t="s">
-        <v>333</v>
-      </c>
-      <c r="BO8" t="s">
-        <v>333</v>
-      </c>
-      <c r="BP8" t="s">
-        <v>333</v>
-      </c>
-      <c r="BQ8" t="s">
-        <v>333</v>
-      </c>
-      <c r="BR8" t="s">
-        <v>333</v>
-      </c>
-      <c r="BS8" t="s">
-        <v>88</v>
-      </c>
-      <c r="BT8" t="s">
-        <v>88</v>
-      </c>
-      <c r="BU8" t="s">
+      <c r="BK8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BL8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BM8" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="BN8" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="BO8" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="BP8" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="BQ8" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="BR8" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="BS8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BU8" s="2" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3159,221 +3137,221 @@
       <c r="A9" t="s">
         <v>79</v>
       </c>
-      <c r="B9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" t="s">
-        <v>120</v>
-      </c>
-      <c r="H9" t="s">
-        <v>127</v>
-      </c>
-      <c r="I9" t="s">
-        <v>133</v>
-      </c>
-      <c r="J9" t="s">
-        <v>139</v>
-      </c>
-      <c r="K9" t="s">
-        <v>144</v>
-      </c>
-      <c r="L9" t="s">
-        <v>149</v>
-      </c>
-      <c r="M9" t="s">
-        <v>156</v>
-      </c>
-      <c r="N9" t="s">
-        <v>86</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="2">
+        <v>33.1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>30.9</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="P9" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>173</v>
-      </c>
-      <c r="R9" t="s">
-        <v>110</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="P9" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="S9" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="U9" t="s">
-        <v>186</v>
-      </c>
-      <c r="V9" t="s">
-        <v>190</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="U9" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="X9" s="2">
+        <v>10.3</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AG9" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AI9" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ9" s="2">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="AK9" s="2">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="AL9" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AM9" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AN9" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="AO9" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AP9" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="AQ9" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="AR9" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="AS9" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AT9" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU9" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="AV9" s="2">
+        <v>62</v>
+      </c>
+      <c r="AW9" s="2">
+        <v>58.7</v>
+      </c>
+      <c r="AX9" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="AY9" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="AZ9" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="BA9" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="X9" t="s">
-        <v>194</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>86</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>197</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>203</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>204</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>204</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>210</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>210</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>214</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>215</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>218</v>
-      </c>
-      <c r="AK9" t="s">
-        <v>219</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>223</v>
-      </c>
-      <c r="AN9" t="s">
-        <v>227</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>232</v>
-      </c>
-      <c r="AP9" t="s">
-        <v>239</v>
-      </c>
-      <c r="AQ9" t="s">
-        <v>245</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>252</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>259</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>266</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>273</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>280</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>287</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>86</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>300</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>307</v>
-      </c>
-      <c r="BA9" t="s">
-        <v>312</v>
-      </c>
-      <c r="BB9" t="s">
+      <c r="BB9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BC9" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="BC9" t="s">
-        <v>105</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>160</v>
-      </c>
-      <c r="BE9" t="s">
-        <v>200</v>
-      </c>
-      <c r="BF9" t="s">
+      <c r="BD9" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="BE9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="BG9" t="s">
-        <v>325</v>
-      </c>
-      <c r="BH9" t="s">
-        <v>99</v>
-      </c>
-      <c r="BI9" t="s">
-        <v>332</v>
-      </c>
-      <c r="BJ9" t="s">
-        <v>86</v>
-      </c>
-      <c r="BK9" t="s">
-        <v>94</v>
-      </c>
-      <c r="BL9" t="s">
-        <v>94</v>
-      </c>
-      <c r="BM9" t="s">
-        <v>94</v>
-      </c>
-      <c r="BN9" t="s">
-        <v>335</v>
-      </c>
-      <c r="BO9" t="s">
-        <v>335</v>
-      </c>
-      <c r="BP9" t="s">
-        <v>335</v>
-      </c>
-      <c r="BQ9" t="s">
-        <v>335</v>
-      </c>
-      <c r="BR9" t="s">
-        <v>335</v>
-      </c>
-      <c r="BS9" t="s">
-        <v>335</v>
-      </c>
-      <c r="BT9" t="s">
+      <c r="BF9" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="BG9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="BH9" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="BI9" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="BJ9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BL9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BM9" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="BN9" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="BO9" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="BP9" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="BQ9" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="BR9" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="BS9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BU9" t="s">
-        <v>336</v>
+      <c r="BT9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="BU9" s="2">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>